<commit_message>
custom part and data sheets
</commit_message>
<xml_diff>
--- a/Lab6/Lab6_Garg_Joglekar (bill of materials CSV).xlsx
+++ b/Lab6/Lab6_Garg_Joglekar (bill of materials CSV).xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Lab6_Garg_Joglekar (bill of mat" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
   <si>
     <t>Component</t>
   </si>
@@ -232,6 +232,12 @@
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>Total Price</t>
+  </si>
+  <si>
+    <t>2.7 ma</t>
   </si>
 </sst>
 </file>
@@ -1038,10 +1044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1383,6 +1389,9 @@
       <c r="I18">
         <v>1</v>
       </c>
+      <c r="J18" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1490,6 +1499,15 @@
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>71</v>
+      </c>
+      <c r="K31">
+        <f>SUM(K2:K25)</f>
+        <v>11.97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>